<commit_message>
MAJ Events card, à fix (+ events.py)
</commit_message>
<xml_diff>
--- a/LineUpXLS.xlsx
+++ b/LineUpXLS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="213">
   <si>
     <t xml:space="preserve">Artist</t>
   </si>
@@ -307,145 +307,347 @@
     <t xml:space="preserve">Lollapalooza</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fame</t>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fame</t>
   </si>
   <si>
     <t xml:space="preserve">style</t>
   </si>
   <si>
+    <t xml:space="preserve">Saucisse</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arrêt saucisse/paëla à la sortie</t>
   </si>
   <si>
+    <t xml:space="preserve">4 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free from desire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gratuit</t>
   </si>
   <si>
+    <t xml:space="preserve">+ 10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 2 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evenement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vegan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bouffe végan</t>
   </si>
   <si>
+    <t xml:space="preserve">1 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conférence</t>
+  </si>
+  <si>
     <t xml:space="preserve">Conférences climat</t>
   </si>
   <si>
-    <t xml:space="preserve">Smalltown boy à la fin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
+    <t xml:space="preserve">open air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smalltown boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le dernier vinyle se pose sur les platines, la nostalgie monte en reconnaissant la musique, car tu as compris que c’est déjà la fin de soirée.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club -5 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 3 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I Love U So</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un mec te fais de l’oeil, tu commences à discuter avec lui, avec un peu de chance tu repartiras avec son numéro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">festival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gourde</t>
   </si>
   <si>
     <t xml:space="preserve">Gourde offerte</t>
   </si>
   <si>
+    <t xml:space="preserve">Bière</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bière gratuite</t>
   </si>
   <si>
+    <t xml:space="preserve">3 1 2 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goodies</t>
+  </si>
+  <si>
     <t xml:space="preserve">Goudies offert (tatoo)</t>
   </si>
   <si>
+    <t xml:space="preserve">event – 3 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glitter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paillettes</t>
   </si>
   <si>
+    <t xml:space="preserve">+ 1 star artists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coucou</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coucou de loin</t>
   </si>
   <si>
+    <t xml:space="preserve">4 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Croiser quelqu'un de connu (Sandrine Rousseau)</t>
   </si>
   <si>
+    <t xml:space="preserve">4 2 1 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambiance</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ambiance de fou (foule en délire)</t>
   </si>
   <si>
-    <t xml:space="preserve">pause attraction/ palais du rire/ peche aux canards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abba passe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beau temps, soleil et pas trop chaud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barbe à papa par le mec de la sécu</t>
+    <t xml:space="preserve">Photomaton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petite pause entre jabberwoky et bob sinclar, la pêche aux canards t’attends après avoir fais ton 3ème polaroid de l’après-midi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco Queen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La reine du Disco fais chauffer la piste, il s’agit bien évidemment d’Abba.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 2 0 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beau temps, soleil et pas trop chaud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open air – 3 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take me up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le mec de la sécurité t’offres une barbe à papa quelle chance.</t>
   </si>
   <si>
     <t xml:space="preserve">Gagner des places sur insta</t>
   </si>
   <si>
-    <t xml:space="preserve">Malus</t>
+    <t xml:space="preserve">3 2 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gobelets</t>
   </si>
   <si>
     <t xml:space="preserve">Gobelets consigné (perte d'argent)</t>
   </si>
   <si>
-    <t xml:space="preserve">-20000 écocups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déluge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open air profit + 5 stars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barrières police</t>
+    <t xml:space="preserve">-20000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La piscine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca y est les nuages sont de la partie et tu passes la moitié du concert d’Angèle à danser sous la pluie battante.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open air + 5 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t wanna Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tu veux aller danser mais la police en a décidé autrement, des barrière encerclent Thylacine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micro</t>
   </si>
   <si>
     <t xml:space="preserve">Problème de micro</t>
   </si>
   <si>
-    <t xml:space="preserve">-1 artiste random</t>
+    <t xml:space="preserve">-1 artist</t>
   </si>
   <si>
     <t xml:space="preserve">Bière renversée</t>
   </si>
   <si>
-    <t xml:space="preserve">Serré comme des sardines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boites profit + 3 stars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panne de courrant (qqun à pisser sur la multiprise)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragueur relou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vent et froid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burger et sushi à 30 balles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plus de papier dans les toilettes/ queue interminable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evacuation par la police (cf radio cargo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retard de l'artiste (pnl tu connais)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1* pour tous les artistes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plus d'ascenseur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soirée profit + 3 stars</t>
+    <t xml:space="preserve">4 3 2 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les sardines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apparemment plus de place ont été vendue que la capacité maximale du lieu, tu te retrouves écrasé entre 2 couples se galochant langoureusement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">club + 3 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the dark</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">C’est la p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">anne de courrant, quelqu’un a eu la bonne idée de pisser sur la multiprise</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance ton quoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comme à chaque festival, parmis tout les dragueur, il y en a forcément un de bien relou.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sous le vent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le déréglement climatique atteindra même les festivals avec ce soudain vent frais qui te rendra enrhumé le lendemain.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Money for Nothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les soirées dans les endroits les plus classes font valoir de leur réputation et ne se gênent pas à vendre des burger et sushi à plus de 30 €.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quanto Tempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus que 20 min à attendre pour pisser un coup, c’est dommage ça te fais louper la performance de Marc Rebillet !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 2 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rave against the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les open air de radio cargo mettent le feu à la capitale, tellement que la police viens pour te virer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always on a run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A leur grande habitude, PNL se font attendre et mette plus de 20min à commencer leur show au WLG.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 star artists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Never going home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La soirée sur le Toit de la défense était mémorable, malheureusement plus aucun ascenseur ne fonctionne, tu restes bloqué au sommet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event + 3 stars</t>
   </si>
   <si>
     <t xml:space="preserve">Plus de taxi</t>
   </si>
   <si>
-    <t xml:space="preserve">Noctilien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vestiaire trop cher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vérification caleçon</t>
+    <t xml:space="preserve">Le monde attiré par le lollapalooza rend compte de la line up de folie proposé, malheureusement, les taxis ne seront eux, pas au rendez-vous.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travelling without arriving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fin de soirée s’annoncera longue car il est maintenant temps de rentré et seul le noctilien te proposera de t’amener chez toi ce soir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thrift Shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment rentabiliser les soirées gratuites ? Proposer un vestiaire ou tu peux payer 9€ pour un manteau et une écharpe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fouille au corps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tu arrives tellement tôt au Nexus que la sécurité te prends pour une mule et te fouilles jusqu’à vérifier l’intégrité de tes sous-vêtements.</t>
   </si>
   <si>
     <t xml:space="preserve">Styles</t>
@@ -486,7 +688,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -521,13 +723,46 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -564,7 +799,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,6 +836,42 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -614,6 +885,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -624,10 +955,10 @@
   </sheetPr>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B32" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1878,7 +2209,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2461,349 +2792,684 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="34.64"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
+      <c r="A2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0"/>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="12" t="n">
+        <f aca="false">SUMIF(E2:E19,"*0*",D2:D19)</f>
+        <v>30</v>
+      </c>
+      <c r="K3" s="12" t="n">
+        <f aca="false">SUMIF(E20:E37,"*0*",D20:D37)</f>
+        <v>-12</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>3</v>
+      <c r="A4" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">SUMIF(E2:E19,"*1*",D2:D19)</f>
+        <v>38</v>
+      </c>
+      <c r="K4" s="12" t="n">
+        <f aca="false">SUMIF(E20:E37,"*1*",D20:D37)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="0"/>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="12" t="n">
+        <f aca="false">SUMIF(E2:E19,"*2*",D2:D19)</f>
+        <v>39</v>
+      </c>
+      <c r="K5" s="12" t="n">
+        <f aca="false">SUMIF(E20:E37,"*2*",D20:D37)</f>
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="0" t="n">
+        <v>114</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="J6" s="12" t="n">
+        <f aca="false">SUMIF(E2:E19,"*3*",D2:D19)</f>
+        <v>28</v>
+      </c>
+      <c r="K6" s="12" t="n">
+        <f aca="false">SUMIF(E20:E37,"*3*",D20:D37)</f>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>3</v>
+        <v>119</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="14" t="n">
+        <f aca="false">SUMIF(E2:E19,"*4*",D2:D19)</f>
+        <v>18</v>
+      </c>
+      <c r="K7" s="13" t="n">
+        <f aca="false">SUMIF(E20:E37,"*4*",D20:D37)</f>
+        <v>-38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="0"/>
+      <c r="D8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="0"/>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="0"/>
+      <c r="D13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="0"/>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="E15" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="0"/>
+      <c r="D16" s="1" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="0" t="n">
+      <c r="E16" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="0"/>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="0"/>
+      <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>116</v>
+      <c r="E19" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="0" t="n">
+      <c r="A23" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="1" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="0" t="n">
+      <c r="E24" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>-5</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="0" t="n">
+      <c r="E25" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="0" t="n">
+      <c r="E26" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="1" t="n">
         <v>-3</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="0" t="n">
+      <c r="E28" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="1" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="0" t="n">
+      <c r="E30" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D34" s="1" t="n">
         <v>-5</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="0" t="n">
+      <c r="E34" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="1" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>-5</v>
+      <c r="E37" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>-3</v>
-      </c>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>-3</v>
-      </c>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>-1</v>
-      </c>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2831,25 +3497,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>203</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="18" t="n">
         <f aca="false">COUNTIF(Artistes!E2:E49,0)</f>
         <v>8</v>
       </c>
@@ -2860,7 +3526,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>145</v>
+        <v>207</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1</v>
@@ -2870,12 +3536,12 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>2</v>
@@ -2884,14 +3550,14 @@
         <f aca="false">COUNTIF(Artistes!E2:E49,2)</f>
         <v>8</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="18" t="n">
         <f aca="false">COUNTIF(Artistes!G2:G49,0)</f>
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>148</v>
+        <v>210</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>3</v>
@@ -2903,7 +3569,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>149</v>
+        <v>211</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>4</v>
@@ -2915,7 +3581,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>150</v>
+        <v>212</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
MAJ Events card, à test
</commit_message>
<xml_diff>
--- a/LineUpXLS.xlsx
+++ b/LineUpXLS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="214">
   <si>
     <t xml:space="preserve">Artist</t>
   </si>
@@ -310,7 +310,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">events</t>
+    <t xml:space="preserve">event</t>
   </si>
   <si>
     <t xml:space="preserve">effect</t>
@@ -487,6 +487,9 @@
     <t xml:space="preserve">Le mec de la sécurité t’offres une barbe à papa quelle chance.</t>
   </si>
   <si>
+    <t xml:space="preserve">Insta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gagner des places sur insta</t>
   </si>
   <si>
@@ -550,23 +553,7 @@
     <t xml:space="preserve">In the dark</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">C’est la p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">anne de courrant, quelqu’un a eu la bonne idée de pisser sur la multiprise</t>
-    </r>
+    <t xml:space="preserve">C’est la panne de courrant, quelqu’un a eu la bonne idée de pisser sur la multiprise</t>
   </si>
   <si>
     <t xml:space="preserve">Balance ton quoi</t>
@@ -620,7 +607,7 @@
     <t xml:space="preserve">event + 3 stars</t>
   </si>
   <si>
-    <t xml:space="preserve">Plus de taxi</t>
+    <t xml:space="preserve">Joe le taxi</t>
   </si>
   <si>
     <t xml:space="preserve">Le monde attiré par le lollapalooza rend compte de la line up de folie proposé, malheureusement, les taxis ne seront eux, pas au rendez-vous.</t>
@@ -688,7 +675,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -733,22 +720,10 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFC9211E"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -799,7 +774,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -840,35 +815,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2794,27 +2757,27 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="34.64"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="4.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="4.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -2837,7 +2800,6 @@
       <c r="B2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="0"/>
       <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
@@ -2846,13 +2808,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -2861,17 +2823,17 @@
       <c r="E3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="12" t="n">
+      <c r="J3" s="11" t="n">
         <f aca="false">SUMIF(E2:E19,"*0*",D2:D19)</f>
         <v>30</v>
       </c>
-      <c r="K3" s="12" t="n">
+      <c r="K3" s="11" t="n">
         <f aca="false">SUMIF(E20:E37,"*0*",D20:D37)</f>
         <v>-12</v>
       </c>
@@ -2883,24 +2845,23 @@
       <c r="B4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="0"/>
       <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="s">
+      <c r="H4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <f aca="false">SUMIF(E2:E19,"*1*",D2:D19)</f>
         <v>38</v>
       </c>
-      <c r="K4" s="12" t="n">
+      <c r="K4" s="11" t="n">
         <f aca="false">SUMIF(E20:E37,"*1*",D20:D37)</f>
         <v>0</v>
       </c>
@@ -2912,36 +2873,35 @@
       <c r="B5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="0"/>
       <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="12" t="n">
+      <c r="J5" s="11" t="n">
         <f aca="false">SUMIF(E2:E19,"*2*",D2:D19)</f>
         <v>39</v>
       </c>
-      <c r="K5" s="12" t="n">
+      <c r="K5" s="11" t="n">
         <f aca="false">SUMIF(E20:E37,"*2*",D20:D37)</f>
         <v>-28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D6" s="1" t="n">
@@ -2950,46 +2910,45 @@
       <c r="E6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" s="0" t="s">
+      <c r="H6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J6" s="12" t="n">
+      <c r="J6" s="11" t="n">
         <f aca="false">SUMIF(E2:E19,"*3*",D2:D19)</f>
         <v>28</v>
       </c>
-      <c r="K6" s="12" t="n">
+      <c r="K6" s="11" t="n">
         <f aca="false">SUMIF(E20:E37,"*3*",D20:D37)</f>
         <v>-12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="0"/>
       <c r="D7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H7" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="I7" s="13" t="s">
+      <c r="H7" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="J7" s="14" t="n">
+      <c r="J7" s="13" t="n">
         <f aca="false">SUMIF(E2:E19,"*4*",D2:D19)</f>
         <v>18</v>
       </c>
-      <c r="K7" s="13" t="n">
+      <c r="K7" s="12" t="n">
         <f aca="false">SUMIF(E20:E37,"*4*",D20:D37)</f>
         <v>-38</v>
       </c>
@@ -3001,7 +2960,6 @@
       <c r="B8" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="0"/>
       <c r="D8" s="1" t="n">
         <v>3</v>
       </c>
@@ -3016,7 +2974,6 @@
       <c r="B9" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="0"/>
       <c r="D9" s="1" t="n">
         <v>5</v>
       </c>
@@ -3031,7 +2988,7 @@
       <c r="B10" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>130</v>
       </c>
       <c r="D10" s="1" t="n">
@@ -3048,7 +3005,7 @@
       <c r="B11" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D11" s="1" t="n">
@@ -3065,7 +3022,6 @@
       <c r="B12" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="0"/>
       <c r="D12" s="1" t="n">
         <v>1</v>
       </c>
@@ -3080,7 +3036,6 @@
       <c r="B13" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="0"/>
       <c r="D13" s="1" t="n">
         <v>3</v>
       </c>
@@ -3095,7 +3050,6 @@
       <c r="B14" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="0"/>
       <c r="D14" s="1" t="n">
         <v>3</v>
       </c>
@@ -3104,13 +3058,13 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="1" t="n">
@@ -3121,13 +3075,12 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>146</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="0"/>
       <c r="D16" s="1" t="n">
         <v>5</v>
       </c>
@@ -3136,13 +3089,13 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>149</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>151</v>
       </c>
       <c r="D17" s="1" t="n">
@@ -3153,13 +3106,12 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>152</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="0"/>
       <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
@@ -3168,79 +3120,81 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>154</v>
+      </c>
       <c r="B19" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C19" s="0"/>
+        <v>155</v>
+      </c>
       <c r="D19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>159</v>
+      <c r="E20" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
-        <v>160</v>
+      <c r="A21" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="11" t="s">
         <v>164</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3249,227 +3203,221 @@
         <v>125</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C24" s="16"/>
+        <v>169</v>
+      </c>
+      <c r="C24" s="14"/>
       <c r="D24" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>169</v>
+      <c r="E24" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>170</v>
+      <c r="A25" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>173</v>
+      <c r="E25" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="11" t="s">
         <v>175</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
-        <v>176</v>
+      <c r="A27" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="E27" s="0" t="s">
-        <v>159</v>
+      <c r="E27" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>178</v>
+      <c r="A28" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
-        <v>180</v>
+      <c r="A29" s="11" t="s">
+        <v>181</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
-        <v>182</v>
+      <c r="A30" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>184</v>
+      <c r="E30" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
-        <v>185</v>
+      <c r="A31" s="11" t="s">
+        <v>186</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
-        <v>187</v>
+      <c r="A32" s="11" t="s">
+        <v>188</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
-        <v>190</v>
+      <c r="A33" s="11" t="s">
+        <v>191</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="s">
-        <v>193</v>
+      <c r="A34" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>-5</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="s">
-        <v>195</v>
+      <c r="A35" s="11" t="s">
+        <v>196</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>197</v>
+      <c r="E35" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="s">
-        <v>198</v>
+      <c r="A36" s="11" t="s">
+        <v>199</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>-3</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>200</v>
+      <c r="E36" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="s">
-        <v>201</v>
+      <c r="A37" s="10" t="s">
+        <v>202</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="E37" s="0" t="s">
-        <v>184</v>
+      <c r="E37" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
+      <c r="B38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
+      <c r="B39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
+      <c r="B40" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3497,25 +3445,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="15" t="n">
         <f aca="false">COUNTIF(Artistes!E2:E49,0)</f>
         <v>8</v>
       </c>
@@ -3526,7 +3474,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1</v>
@@ -3536,12 +3484,12 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>2</v>
@@ -3550,14 +3498,14 @@
         <f aca="false">COUNTIF(Artistes!E2:E49,2)</f>
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="15" t="n">
         <f aca="false">COUNTIF(Artistes!G2:G49,0)</f>
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>3</v>
@@ -3569,7 +3517,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>4</v>
@@ -3581,7 +3529,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>5</v>

</xml_diff>